<commit_message>
Update in WBS, please fill the fields relevant to your tasks
</commit_message>
<xml_diff>
--- a/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
+++ b/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>nr</t>
   </si>
@@ -142,13 +142,28 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Automatish opslaan of via save button</t>
+  </si>
+  <si>
+    <t>1,5 = ander half uur</t>
+  </si>
+  <si>
+    <t>Dus niet 1 uur en 5 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +210,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,6 +338,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -593,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -711,6 +744,9 @@
       <c r="D4" s="13" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
@@ -732,6 +768,12 @@
       <c r="C5" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -753,6 +795,12 @@
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
@@ -774,6 +822,12 @@
       <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
@@ -795,6 +849,12 @@
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
@@ -816,6 +876,9 @@
       <c r="C9" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D9" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
@@ -837,6 +900,9 @@
       <c r="C10" s="24" t="s">
         <v>7</v>
       </c>
+      <c r="D10" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
@@ -858,6 +924,9 @@
       <c r="C11" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
@@ -879,6 +948,9 @@
       <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D12" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
@@ -900,6 +972,9 @@
       <c r="C13" s="24" t="s">
         <v>7</v>
       </c>
+      <c r="D13" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
@@ -921,6 +996,9 @@
       <c r="C14" s="24" t="s">
         <v>11</v>
       </c>
+      <c r="D14" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
@@ -941,6 +1019,9 @@
       </c>
       <c r="C15" s="24" t="s">
         <v>11</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
@@ -980,7 +1061,7 @@
       <c r="E17" s="21"/>
       <c r="F17" s="2">
         <f>SUBTOTAL(9,F4:F16)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2">
         <f>SUBTOTAL(9,G4:G16)</f>
@@ -998,6 +1079,19 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E20" s="25"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E24" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E25" s="26" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:I11"/>

</xml_diff>

<commit_message>
Finished Work break down structure
</commit_message>
<xml_diff>
--- a/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
+++ b/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
@@ -16,7 +16,7 @@
     <sheet name="MoSCoW" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">projectnaam!$A$3:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">projectnaam!$A$3:$I$27</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>nr</t>
   </si>
@@ -157,6 +157,45 @@
   </si>
   <si>
     <t>Dus niet 1 uur en 5 min</t>
+  </si>
+  <si>
+    <t>Check if you can add unlimited Projects</t>
+  </si>
+  <si>
+    <t>Check if you can add unlimited Tasks</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>Responsive maintenance</t>
+  </si>
+  <si>
+    <t>Clean up code, make code efficient</t>
+  </si>
+  <si>
+    <t>Clean up file structure, orginize files</t>
+  </si>
+  <si>
+    <t>Form validation</t>
+  </si>
+  <si>
+    <t>User feedback (messages)</t>
+  </si>
+  <si>
+    <t>If plan &gt; do Give a red color</t>
+  </si>
+  <si>
+    <t>If total plan &gt; do Give color</t>
+  </si>
+  <si>
+    <t>Test website (different browsers)</t>
+  </si>
+  <si>
+    <t>Database maintenance</t>
+  </si>
+  <si>
+    <t>Kevin &amp; Damien</t>
   </si>
 </sst>
 </file>
@@ -277,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -338,9 +377,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -626,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -739,7 +775,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>26</v>
@@ -796,10 +832,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.5</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -946,7 +985,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>39</v>
@@ -994,7 +1033,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>39</v>
@@ -1018,7 +1057,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>39</v>
@@ -1038,8 +1077,18 @@
       <c r="A16" s="24">
         <v>13</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.25</v>
+      </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
@@ -1052,23 +1101,21 @@
       <c r="S16" s="22"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="2">
-        <f>SUBTOTAL(9,F4:F16)</f>
-        <v>6</v>
-      </c>
-      <c r="G17" s="2">
-        <f>SUBTOTAL(9,G4:G16)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="A17" s="24">
+        <v>14</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.25</v>
+      </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
@@ -1080,21 +1127,293 @@
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
     </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>15</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>16</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+    </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E20" s="25"/>
+      <c r="A20" s="24">
+        <v>17</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>18</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>19</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>20</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E24" s="26" t="s">
+      <c r="A24" s="24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>22</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="24">
+        <v>23</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="24">
+        <v>24</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="2">
+        <f>SUBTOTAL(9,F4:F21)</f>
+        <v>15</v>
+      </c>
+      <c r="G28" s="2">
+        <f>SUBTOTAL(9,G4:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E30" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E25" s="26" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E31" s="25" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A3:I11"/>
+  <autoFilter ref="A3:I27"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Work break down structure (for real)
</commit_message>
<xml_diff>
--- a/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
+++ b/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>nr</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Kevin &amp; Damien</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -865,10 +868,10 @@
         <v>11</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -921,6 +924,9 @@
       <c r="D9" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
@@ -945,6 +951,9 @@
       <c r="D10" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
@@ -969,6 +978,9 @@
       <c r="D11" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
@@ -993,6 +1005,9 @@
       <c r="D12" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="F12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
@@ -1017,6 +1032,9 @@
       <c r="D13" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
@@ -1041,6 +1059,9 @@
       <c r="D14" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="F14" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
@@ -1065,6 +1086,9 @@
       <c r="D15" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="F15" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
@@ -1248,6 +1272,12 @@
       <c r="C22" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D22" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
@@ -1269,6 +1299,12 @@
       <c r="C23" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
@@ -1290,6 +1326,12 @@
       <c r="C24" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
@@ -1311,6 +1353,12 @@
       <c r="C25" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
@@ -1332,6 +1380,12 @@
       <c r="C26" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
@@ -1353,6 +1407,12 @@
       <c r="C27" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
@@ -1373,8 +1433,8 @@
       <c r="D28" s="14"/>
       <c r="E28" s="21"/>
       <c r="F28" s="2">
-        <f>SUBTOTAL(9,F4:F21)</f>
-        <v>15</v>
+        <f>SUBTOTAL(9,F4:F27)</f>
+        <v>34</v>
       </c>
       <c r="G28" s="2">
         <f>SUBTOTAL(9,G4:G17)</f>

</xml_diff>

<commit_message>
Worked on display time, Created folder 'functions' to store php functions.
</commit_message>
<xml_diff>
--- a/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
+++ b/documents/workbreakdown - WBSMonitor - WD - 1- ict college.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>nr</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>begonnen: 15:55 -16:57</t>
   </si>
 </sst>
 </file>
@@ -665,10 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -770,7 +774,7 @@
       <c r="R3" s="23"/>
       <c r="S3" s="23"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>1</v>
       </c>
@@ -857,7 +861,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -900,6 +904,12 @@
       <c r="F8" s="1">
         <v>1.5</v>
       </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
@@ -911,7 +921,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>6</v>
       </c>
@@ -938,7 +948,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>7</v>
       </c>
@@ -965,7 +975,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>8</v>
       </c>
@@ -992,7 +1002,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <v>9</v>
       </c>
@@ -1019,7 +1029,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>10</v>
       </c>
@@ -1046,7 +1056,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>11</v>
       </c>
@@ -1073,7 +1083,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>12</v>
       </c>
@@ -1100,7 +1110,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>13</v>
       </c>
@@ -1127,7 +1137,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>14</v>
       </c>
@@ -1154,7 +1164,7 @@
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>15</v>
       </c>
@@ -1181,7 +1191,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>16</v>
       </c>
@@ -1208,7 +1218,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>17</v>
       </c>
@@ -1235,7 +1245,7 @@
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <v>18</v>
       </c>
@@ -1262,7 +1272,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24">
         <v>19</v>
       </c>
@@ -1289,7 +1299,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <v>20</v>
       </c>
@@ -1316,7 +1326,7 @@
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
         <v>21</v>
       </c>
@@ -1343,7 +1353,7 @@
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
         <v>22</v>
       </c>
@@ -1370,7 +1380,7 @@
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
         <v>23</v>
       </c>
@@ -1397,7 +1407,7 @@
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
         <v>24</v>
       </c>
@@ -1434,11 +1444,11 @@
       <c r="E28" s="21"/>
       <c r="F28" s="2">
         <f>SUBTOTAL(9,F4:F27)</f>
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="G28" s="2">
         <f>SUBTOTAL(9,G4:G17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1476,7 +1486,19 @@
       <c r="E36" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:I27"/>
+  <autoFilter ref="A3:I27">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="M"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Damien"/>
+        <filter val="Kevin &amp; Damien"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>